<commit_message>
Inclusión de sección Competencias
Inclusión de sección Competencias
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion09/EsqueletoGuion_CN_11_09_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion09/EsqueletoGuion_CN_11_09_CO.xlsx
@@ -19,7 +19,7 @@
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$A$1:$C$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$A$1:$C$24</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="100">
   <si>
     <t>FICHA</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t xml:space="preserve">Evaluación </t>
+  </si>
+  <si>
+    <t>Competencias: cantidad de bicarbonato en un antiácido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competencias: cantidad de bicarbonato en un antiácido </t>
+  </si>
+  <si>
+    <t>Competencias</t>
   </si>
 </sst>
 </file>
@@ -887,7 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1029,6 +1038,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1790,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2127,26 @@
         <v>18</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="16">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2124,7 +2163,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,7 +2257,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="13">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,7 +2268,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="13">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2257,10 +2296,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,15 +2540,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>43</v>
+      <c r="B22" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="64" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,14 +2556,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="6"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>23</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2532,7 +2582,7 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -2543,11 +2593,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,41 +4885,79 @@
         <v>43</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B115" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C115" s="14"/>
+      <c r="B115" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="D115" s="15"/>
       <c r="E115" s="15"/>
       <c r="F115" s="15"/>
       <c r="G115" s="15"/>
-      <c r="H115" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I115" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H115" s="65"/>
+      <c r="I115" s="66"/>
+    </row>
+    <row r="116" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B116" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C116" s="14"/>
+      <c r="B116" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="D116" s="15"/>
       <c r="E116" s="15"/>
       <c r="F116" s="15"/>
       <c r="G116" s="15"/>
-      <c r="H116" s="16" t="s">
+      <c r="H116" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="I116" s="66" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C117" s="14"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I117" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C118" s="14"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I116" s="16" t="s">
+      <c r="I118" s="16" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>